<commit_message>
Committ after glo_cds change
</commit_message>
<xml_diff>
--- a/Data/Oil_price_effect_own_calculation.xlsx
+++ b/Data/Oil_price_effect_own_calculation.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timodaehler/Desktop/COVID19-DOMINANCE/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1362F7-75B9-724F-8075-C0154BB3D38F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B899133-B8B4-AB4F-B176-55E28DB88FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{622DD5D3-366B-554D-807D-ACB27C68A51A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{622DD5D3-366B-554D-807D-ACB27C68A51A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="RAW DATA" sheetId="1" r:id="rId1"/>
+    <sheet name="R" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="193">
   <si>
     <t>TOTAL_EXPORT_2018</t>
   </si>
@@ -606,7 +606,13 @@
     <t>Czechia</t>
   </si>
   <si>
-    <t>Oil</t>
+    <t>These are the values that are copied into the sheet "paneladdition"</t>
+  </si>
+  <si>
+    <t>Oil effect before price interaction</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
   </si>
 </sst>
 </file>
@@ -654,7 +660,7 @@
       <name val="MetaWebPro"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,6 +676,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -715,6 +727,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,9 +1045,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49B1146-0CFB-5E4B-8A5D-B91D4BC1DE41}">
   <dimension ref="A1:AA158"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A42" sqref="A42"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1688,7 +1701,7 @@
         <v>0.16419928411913698</v>
       </c>
       <c r="V7" s="10">
-        <f t="shared" ref="V3:V65" si="15">Q7*M7*D7</f>
+        <f t="shared" ref="V7:V65" si="15">Q7*M7*D7</f>
         <v>-2.6916349785676488E-3</v>
       </c>
       <c r="W7" s="12">
@@ -16434,10 +16447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C639D427-C41A-1B45-B1EF-B1810A867248}">
-  <dimension ref="A1:J159"/>
+  <dimension ref="A1:O159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -16449,7 +16462,7 @@
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:15">
       <c r="A1">
         <v>1</v>
       </c>
@@ -16469,7 +16482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>183</v>
       </c>
@@ -16489,13 +16502,13 @@
         <v>184</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
@@ -16522,8 +16535,15 @@
         <f>VLOOKUP(I3,$A$3:$F$157,6,FALSE)</f>
         <v>-8.6035798144359944E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -16547,11 +16567,11 @@
         <v>35</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J36" si="1">VLOOKUP(I4,$A$3:$F$157,6,FALSE)</f>
+        <f t="shared" ref="J4:J35" si="1">VLOOKUP(I4,$A$3:$F$157,6,FALSE)</f>
         <v>0.47420548262690787</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:15">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -16579,7 +16599,7 @@
         <v>0.17263287353225784</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:15">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -16607,7 +16627,7 @@
         <v>-2.5844567624387117E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:15">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -16635,7 +16655,7 @@
         <v>-4.81736030198089E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:15">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -16652,7 +16672,7 @@
         <v>0.16419928411913698</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>B8*D8-C8*E8</f>
         <v>-8.6035798144359944E-3</v>
       </c>
       <c r="I8" t="s">
@@ -16663,7 +16683,7 @@
         <v>-2.686431820487482E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:15">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -16691,7 +16711,7 @@
         <v>7.7758537294080859E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:15">
       <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
@@ -16719,7 +16739,7 @@
         <v>-5.2578777079730535E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:15">
       <c r="A11" s="6" t="s">
         <v>35</v>
       </c>
@@ -16747,7 +16767,7 @@
         <v>-4.7907038910496025E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17">
+    <row r="12" spans="1:15" ht="17">
       <c r="A12" s="7" t="s">
         <v>36</v>
       </c>
@@ -16775,7 +16795,7 @@
         <v>0.10039812454475661</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:15">
       <c r="A13" s="6" t="s">
         <v>37</v>
       </c>
@@ -16803,7 +16823,7 @@
         <v>-3.9519855874762866E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:15">
       <c r="A14" s="6" t="s">
         <v>38</v>
       </c>
@@ -16831,7 +16851,7 @@
         <v>1.1963391037637772E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:15">
       <c r="A15" s="6" t="s">
         <v>39</v>
       </c>
@@ -16859,7 +16879,7 @@
         <v>0.24955471251717934</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:15">
       <c r="A16" s="6" t="s">
         <v>40</v>
       </c>

</xml_diff>